<commit_message>
03 27 probaerettsegi2 #2
</commit_message>
<xml_diff>
--- a/Kadarkuti_Marton/_ERETTSEGI_GYAKR/probaerettsegi0325/ballagas.xlsx
+++ b/Kadarkuti_Marton/_ERETTSEGI_GYAKR/probaerettsegi0325/ballagas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\merkur07\fakt2023\Kadarkuti_Marton\_ERETTSEGI_GYAKR\probaerettsegi0325\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14320BA8-8828-4B32-B281-028A60DECCFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590D3F82-D36D-4638-ACFB-3277BBD4D948}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9225" xr2:uid="{5634BA4D-864B-44F9-95B7-712BF75FB2BC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9225" activeTab="1" xr2:uid="{5634BA4D-864B-44F9-95B7-712BF75FB2BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Válaszok" sheetId="1" r:id="rId1"/>
@@ -312,8 +312,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="170" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="General&quot;. helyen&quot;"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="General&quot;. helyen&quot;"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -334,7 +334,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,6 +344,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -375,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -383,10 +389,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -396,53 +402,26 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color theme="9"/>
@@ -775,9 +754,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3EFCC5F-6386-4155-85A6-1CD7AAB07DC0}">
   <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K8" sqref="K8"/>
+      <selection pane="topRight" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1814,7 +1793,7 @@
         <v>7</v>
       </c>
       <c r="J19" s="7" t="str">
-        <f t="shared" ref="J19:P71" si="2">IFERROR(SEARCH(J$1,$I19),"")</f>
+        <f t="shared" ref="J19:P55" si="2">IFERROR(SEARCH(J$1,$I19),"")</f>
         <v/>
       </c>
       <c r="K19" s="7" t="str">
@@ -4901,21 +4880,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DCF652-47BD-4B46-AB34-4511029C9A6B}">
   <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" style="14" customWidth="1"/>
     <col min="2" max="8" width="5.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="23.7109375" customWidth="1"/>
     <col min="10" max="16" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -4965,7 +4944,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="5">
@@ -5022,7 +5001,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="5">
@@ -5079,7 +5058,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="10" t="s">
         <v>55</v>
       </c>
       <c r="B4" s="5">
@@ -5136,7 +5115,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B5" s="5">
@@ -5193,7 +5172,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="10" t="s">
         <v>62</v>
       </c>
       <c r="B6" s="5">
@@ -5248,7 +5227,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="10" t="s">
         <v>67</v>
       </c>
       <c r="B7" s="5">
@@ -5305,7 +5284,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="5">
@@ -5360,7 +5339,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="5">
@@ -5415,7 +5394,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="5">
@@ -5472,7 +5451,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="5">
@@ -5527,7 +5506,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="15" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="5">
@@ -5584,7 +5563,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="16" t="s">
         <v>54</v>
       </c>
       <c r="B13" s="5">
@@ -5639,32 +5618,32 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>69</v>
+      <c r="A14" s="16" t="s">
+        <v>70</v>
       </c>
       <c r="B14" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D14" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F14" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G14" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H14" s="5">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J14" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I14),"")</f>
@@ -5678,13 +5657,13 @@
         <f>IFERROR(SEARCH(L$1,$I14),"")</f>
         <v/>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="7" t="str">
         <f>IFERROR(SEARCH(M$1,$I14),"")</f>
-        <v>1</v>
-      </c>
-      <c r="N14" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N14" s="7">
         <f>IFERROR(SEARCH(N$1,$I14),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="O14" s="7" t="str">
         <f>IFERROR(SEARCH(O$1,$I14),"")</f>
@@ -5696,26 +5675,26 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>11</v>
+      <c r="A15" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="B15" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D15" s="5">
         <v>3</v>
       </c>
       <c r="E15" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F15" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G15" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H15" s="5">
         <v>2</v>
@@ -5751,23 +5730,23 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>12</v>
+      <c r="A16" s="16" t="s">
+        <v>72</v>
       </c>
       <c r="B16" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C16" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D16" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F16" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G16" s="5">
         <v>5</v>
@@ -5775,7 +5754,9 @@
       <c r="H16" s="5">
         <v>2</v>
       </c>
-      <c r="I16" s="7"/>
+      <c r="I16" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="J16" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I16),"")</f>
         <v/>
@@ -5792,9 +5773,9 @@
         <f>IFERROR(SEARCH(M$1,$I16),"")</f>
         <v/>
       </c>
-      <c r="N16" s="7" t="str">
+      <c r="N16" s="7">
         <f>IFERROR(SEARCH(N$1,$I16),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="O16" s="7" t="str">
         <f>IFERROR(SEARCH(O$1,$I16),"")</f>
@@ -5806,31 +5787,33 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>41</v>
+      <c r="A17" s="16" t="s">
+        <v>83</v>
       </c>
       <c r="B17" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C17" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D17" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E17" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G17" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H17" s="5">
         <v>2</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="J17" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I17),"")</f>
         <v/>
@@ -5847,45 +5830,47 @@
         <f>IFERROR(SEARCH(M$1,$I17),"")</f>
         <v/>
       </c>
-      <c r="N17" s="7" t="str">
+      <c r="N17" s="7">
         <f>IFERROR(SEARCH(N$1,$I17),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="O17" s="7" t="str">
         <f>IFERROR(SEARCH(O$1,$I17),"")</f>
         <v/>
       </c>
-      <c r="P17" s="7" t="str">
+      <c r="P17" s="7">
         <f>IFERROR(SEARCH(P$1,$I17),"")</f>
-        <v/>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>52</v>
+      <c r="A18" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="B18" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D18" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E18" s="5">
         <v>2</v>
       </c>
       <c r="F18" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G18" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H18" s="5">
-        <v>1</v>
-      </c>
-      <c r="I18" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="J18" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I18),"")</f>
         <v/>
@@ -5898,13 +5883,13 @@
         <f>IFERROR(SEARCH(L$1,$I18),"")</f>
         <v/>
       </c>
-      <c r="M18" s="7" t="str">
+      <c r="M18" s="7">
         <f>IFERROR(SEARCH(M$1,$I18),"")</f>
-        <v/>
-      </c>
-      <c r="N18" s="7" t="str">
+        <v>12</v>
+      </c>
+      <c r="N18" s="7">
         <f>IFERROR(SEARCH(N$1,$I18),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="O18" s="7" t="str">
         <f>IFERROR(SEARCH(O$1,$I18),"")</f>
@@ -5916,32 +5901,32 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>70</v>
+      <c r="A19" s="16" t="s">
+        <v>57</v>
       </c>
       <c r="B19" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D19" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E19" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" s="5">
         <v>1</v>
       </c>
       <c r="G19" s="5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H19" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="J19" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I19),"")</f>
@@ -5963,9 +5948,9 @@
         <f>IFERROR(SEARCH(N$1,$I19),"")</f>
         <v>1</v>
       </c>
-      <c r="O19" s="7" t="str">
+      <c r="O19" s="7">
         <f>IFERROR(SEARCH(O$1,$I19),"")</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="P19" s="7" t="str">
         <f>IFERROR(SEARCH(P$1,$I19),"")</f>
@@ -5973,20 +5958,20 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>71</v>
+      <c r="A20" s="16" t="s">
+        <v>75</v>
       </c>
       <c r="B20" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D20" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E20" s="5">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F20" s="5">
         <v>1</v>
@@ -5995,7 +5980,7 @@
         <v>7</v>
       </c>
       <c r="H20" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="7" t="str">
@@ -6028,36 +6013,34 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>17</v>
+      <c r="A21" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="B21" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C21" s="5">
         <v>5</v>
       </c>
       <c r="D21" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E21" s="5">
         <v>3</v>
       </c>
       <c r="F21" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G21" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H21" s="5">
-        <v>1</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="7">
+        <v>2</v>
+      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I21),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="K21" s="7" t="str">
         <f>IFERROR(SEARCH(K$1,$I21),"")</f>
@@ -6079,38 +6062,38 @@
         <f>IFERROR(SEARCH(O$1,$I21),"")</f>
         <v/>
       </c>
-      <c r="P21" s="7">
+      <c r="P21" s="7" t="str">
         <f>IFERROR(SEARCH(P$1,$I21),"")</f>
-        <v>15</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>26</v>
+      <c r="A22" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="B22" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D22" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E22" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F22" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G22" s="5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H22" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J22" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I22),"")</f>
@@ -6124,13 +6107,13 @@
         <f>IFERROR(SEARCH(L$1,$I22),"")</f>
         <v/>
       </c>
-      <c r="M22" s="7">
+      <c r="M22" s="7" t="str">
         <f>IFERROR(SEARCH(M$1,$I22),"")</f>
-        <v>1</v>
-      </c>
-      <c r="N22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N22" s="7">
         <f>IFERROR(SEARCH(N$1,$I22),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="O22" s="7" t="str">
         <f>IFERROR(SEARCH(O$1,$I22),"")</f>
@@ -6142,33 +6125,31 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>30</v>
+      <c r="A23" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="B23" s="5">
         <v>5</v>
       </c>
       <c r="C23" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D23" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E23" s="5">
         <v>3</v>
       </c>
       <c r="F23" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G23" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H23" s="5">
-        <v>1</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>7</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I23" s="7"/>
       <c r="J23" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I23),"")</f>
         <v/>
@@ -6193,42 +6174,42 @@
         <f>IFERROR(SEARCH(O$1,$I23),"")</f>
         <v/>
       </c>
-      <c r="P23" s="7">
+      <c r="P23" s="7" t="str">
         <f>IFERROR(SEARCH(P$1,$I23),"")</f>
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>44</v>
+      <c r="A24" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="B24" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C24" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E24" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G24" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H24" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J24" s="7">
+        <v>5</v>
+      </c>
+      <c r="J24" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I24),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="K24" s="7" t="str">
         <f>IFERROR(SEARCH(K$1,$I24),"")</f>
@@ -6242,9 +6223,9 @@
         <f>IFERROR(SEARCH(M$1,$I24),"")</f>
         <v/>
       </c>
-      <c r="N24" s="7" t="str">
+      <c r="N24" s="7">
         <f>IFERROR(SEARCH(N$1,$I24),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="O24" s="7" t="str">
         <f>IFERROR(SEARCH(O$1,$I24),"")</f>
@@ -6256,29 +6237,29 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>50</v>
+      <c r="A25" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="B25" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C25" s="5">
         <v>2</v>
       </c>
       <c r="D25" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E25" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F25" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G25" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H25" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="7" t="str">
@@ -6311,26 +6292,26 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>65</v>
+      <c r="A26" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="B26" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C26" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D26" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E26" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F26" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G26" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H26" s="5">
         <v>6</v>
@@ -6366,17 +6347,17 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>72</v>
+      <c r="A27" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="B27" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C27" s="5">
         <v>6</v>
       </c>
       <c r="D27" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E27" s="5">
         <v>3</v>
@@ -6385,14 +6366,12 @@
         <v>1</v>
       </c>
       <c r="G27" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H27" s="5">
         <v>2</v>
       </c>
-      <c r="I27" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="I27" s="7"/>
       <c r="J27" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I27),"")</f>
         <v/>
@@ -6409,9 +6388,9 @@
         <f>IFERROR(SEARCH(M$1,$I27),"")</f>
         <v/>
       </c>
-      <c r="N27" s="7">
+      <c r="N27" s="7" t="str">
         <f>IFERROR(SEARCH(N$1,$I27),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="O27" s="7" t="str">
         <f>IFERROR(SEARCH(O$1,$I27),"")</f>
@@ -6423,33 +6402,31 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>83</v>
+      <c r="A28" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="B28" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D28" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E28" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F28" s="5">
         <v>1</v>
       </c>
       <c r="G28" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H28" s="5">
         <v>2</v>
       </c>
-      <c r="I28" s="7" t="s">
-        <v>84</v>
-      </c>
+      <c r="I28" s="7"/>
       <c r="J28" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I28),"")</f>
         <v/>
@@ -6466,43 +6443,43 @@
         <f>IFERROR(SEARCH(M$1,$I28),"")</f>
         <v/>
       </c>
-      <c r="N28" s="7">
+      <c r="N28" s="7" t="str">
         <f>IFERROR(SEARCH(N$1,$I28),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="O28" s="7" t="str">
         <f>IFERROR(SEARCH(O$1,$I28),"")</f>
         <v/>
       </c>
-      <c r="P28" s="7">
+      <c r="P28" s="7" t="str">
         <f>IFERROR(SEARCH(P$1,$I28),"")</f>
-        <v>12</v>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>85</v>
+      <c r="A29" s="11" t="s">
+        <v>68</v>
       </c>
       <c r="B29" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29" s="5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D29" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E29" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F29" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G29" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H29" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I29" s="7"/>
       <c r="J29" s="7" t="str">
@@ -6535,29 +6512,29 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>87</v>
+      <c r="A30" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="B30" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C30" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D30" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E30" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F30" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G30" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H30" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I30" s="7"/>
       <c r="J30" s="7" t="str">
@@ -6590,7 +6567,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="11" t="s">
         <v>90</v>
       </c>
       <c r="B31" s="5">
@@ -6647,31 +6624,33 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>19</v>
+      <c r="A32" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="B32" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C32" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32" s="5">
         <v>5</v>
       </c>
       <c r="E32" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F32" s="5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G32" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H32" s="5">
         <v>1</v>
       </c>
-      <c r="I32" s="7"/>
+      <c r="I32" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="J32" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I32),"")</f>
         <v/>
@@ -6696,38 +6675,38 @@
         <f>IFERROR(SEARCH(O$1,$I32),"")</f>
         <v/>
       </c>
-      <c r="P32" s="7" t="str">
+      <c r="P32" s="7">
         <f>IFERROR(SEARCH(P$1,$I32),"")</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>23</v>
+      <c r="A33" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="B33" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C33" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D33" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E33" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G33" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H33" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="J33" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I33),"")</f>
@@ -6743,11 +6722,11 @@
       </c>
       <c r="M33" s="7">
         <f>IFERROR(SEARCH(M$1,$I33),"")</f>
-        <v>12</v>
-      </c>
-      <c r="N33" s="7">
+        <v>1</v>
+      </c>
+      <c r="N33" s="7" t="str">
         <f>IFERROR(SEARCH(N$1,$I33),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="O33" s="7" t="str">
         <f>IFERROR(SEARCH(O$1,$I33),"")</f>
@@ -6759,40 +6738,38 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>28</v>
+      <c r="A34" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="B34" s="5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C34" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D34" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E34" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F34" s="5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G34" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H34" s="5">
-        <v>6</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>2</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="I34" s="7"/>
       <c r="J34" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I34),"")</f>
         <v/>
       </c>
-      <c r="K34" s="7">
+      <c r="K34" s="7" t="str">
         <f>IFERROR(SEARCH(K$1,$I34),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="L34" s="7" t="str">
         <f>IFERROR(SEARCH(L$1,$I34),"")</f>
@@ -6816,40 +6793,38 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>39</v>
+      <c r="A35" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="B35" s="5">
         <v>3</v>
       </c>
       <c r="C35" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D35" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E35" s="5">
         <v>6</v>
       </c>
       <c r="F35" s="5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G35" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H35" s="5">
-        <v>2</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>40</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I35" s="7"/>
       <c r="J35" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I35),"")</f>
         <v/>
       </c>
-      <c r="K35" s="7">
+      <c r="K35" s="7" t="str">
         <f>IFERROR(SEARCH(K$1,$I35),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="L35" s="7" t="str">
         <f>IFERROR(SEARCH(L$1,$I35),"")</f>
@@ -6867,38 +6842,38 @@
         <f>IFERROR(SEARCH(O$1,$I35),"")</f>
         <v/>
       </c>
-      <c r="P35" s="7">
+      <c r="P35" s="7" t="str">
         <f>IFERROR(SEARCH(P$1,$I35),"")</f>
-        <v>10</v>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
-        <v>64</v>
+      <c r="A36" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="B36" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C36" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D36" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E36" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F36" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G36" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H36" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J36" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I36),"")</f>
@@ -6912,9 +6887,9 @@
         <f>IFERROR(SEARCH(L$1,$I36),"")</f>
         <v/>
       </c>
-      <c r="M36" s="7" t="str">
+      <c r="M36" s="7">
         <f>IFERROR(SEARCH(M$1,$I36),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="N36" s="7" t="str">
         <f>IFERROR(SEARCH(N$1,$I36),"")</f>
@@ -6924,35 +6899,35 @@
         <f>IFERROR(SEARCH(O$1,$I36),"")</f>
         <v/>
       </c>
-      <c r="P36" s="7">
+      <c r="P36" s="7" t="str">
         <f>IFERROR(SEARCH(P$1,$I36),"")</f>
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
-        <v>15</v>
+      <c r="A37" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="B37" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D37" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E37" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" s="5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G37" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H37" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7" t="str">
@@ -6985,32 +6960,32 @@
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>34</v>
+      <c r="A38" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="B38" s="5">
         <v>2</v>
       </c>
       <c r="C38" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D38" s="5">
         <v>6</v>
       </c>
       <c r="E38" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F38" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G38" s="5">
         <v>5</v>
       </c>
       <c r="H38" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="J38" s="7">
         <f>IFERROR(SEARCH(J$1,$I38),"")</f>
@@ -7024,9 +6999,9 @@
         <f>IFERROR(SEARCH(L$1,$I38),"")</f>
         <v/>
       </c>
-      <c r="M38" s="7" t="str">
+      <c r="M38" s="7">
         <f>IFERROR(SEARCH(M$1,$I38),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="N38" s="7" t="str">
         <f>IFERROR(SEARCH(N$1,$I38),"")</f>
@@ -7036,40 +7011,42 @@
         <f>IFERROR(SEARCH(O$1,$I38),"")</f>
         <v/>
       </c>
-      <c r="P38" s="7">
+      <c r="P38" s="7" t="str">
         <f>IFERROR(SEARCH(P$1,$I38),"")</f>
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
-        <v>45</v>
+      <c r="A39" s="11" t="s">
+        <v>89</v>
       </c>
       <c r="B39" s="5">
         <v>1</v>
       </c>
       <c r="C39" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D39" s="5">
         <v>6</v>
       </c>
       <c r="E39" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F39" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G39" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H39" s="5">
-        <v>3</v>
-      </c>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7" t="str">
+        <v>2</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J39" s="7">
         <f>IFERROR(SEARCH(J$1,$I39),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="K39" s="7" t="str">
         <f>IFERROR(SEARCH(K$1,$I39),"")</f>
@@ -7091,39 +7068,37 @@
         <f>IFERROR(SEARCH(O$1,$I39),"")</f>
         <v/>
       </c>
-      <c r="P39" s="7" t="str">
+      <c r="P39" s="7">
         <f>IFERROR(SEARCH(P$1,$I39),"")</f>
-        <v/>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>47</v>
+      <c r="A40" s="11" t="s">
+        <v>27</v>
       </c>
       <c r="B40" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C40" s="5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D40" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E40" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G40" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H40" s="5">
-        <v>1</v>
-      </c>
-      <c r="I40" s="7" t="s">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="I40" s="7"/>
       <c r="J40" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I40),"")</f>
         <v/>
@@ -7148,46 +7123,46 @@
         <f>IFERROR(SEARCH(O$1,$I40),"")</f>
         <v/>
       </c>
-      <c r="P40" s="7">
+      <c r="P40" s="7" t="str">
         <f>IFERROR(SEARCH(P$1,$I40),"")</f>
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>57</v>
+      <c r="A41" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="B41" s="5">
         <v>3</v>
       </c>
       <c r="C41" s="5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D41" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E41" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F41" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G41" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H41" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="J41" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I41),"")</f>
         <v/>
       </c>
-      <c r="K41" s="7" t="str">
+      <c r="K41" s="7">
         <f>IFERROR(SEARCH(K$1,$I41),"")</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="L41" s="7" t="str">
         <f>IFERROR(SEARCH(L$1,$I41),"")</f>
@@ -7197,43 +7172,43 @@
         <f>IFERROR(SEARCH(M$1,$I41),"")</f>
         <v/>
       </c>
-      <c r="N41" s="7">
+      <c r="N41" s="7" t="str">
         <f>IFERROR(SEARCH(N$1,$I41),"")</f>
-        <v>1</v>
-      </c>
-      <c r="O41" s="7">
+        <v/>
+      </c>
+      <c r="O41" s="7" t="str">
         <f>IFERROR(SEARCH(O$1,$I41),"")</f>
-        <v>12</v>
-      </c>
-      <c r="P41" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P41" s="7">
         <f>IFERROR(SEARCH(P$1,$I41),"")</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>74</v>
+      <c r="A42" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="B42" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C42" s="5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D42" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E42" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F42" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G42" s="5">
         <v>4</v>
       </c>
       <c r="H42" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I42" s="7"/>
       <c r="J42" s="7" t="str">
@@ -7266,29 +7241,29 @@
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
-        <v>75</v>
+      <c r="A43" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="B43" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C43" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D43" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E43" s="5">
         <v>2</v>
       </c>
       <c r="F43" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G43" s="5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H43" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I43" s="7"/>
       <c r="J43" s="7" t="str">
@@ -7321,34 +7296,36 @@
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
-        <v>76</v>
+      <c r="A44" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="B44" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C44" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D44" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E44" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F44" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G44" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H44" s="5">
-        <v>3</v>
-      </c>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7" t="str">
+        <v>6</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J44" s="7">
         <f>IFERROR(SEARCH(J$1,$I44),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="K44" s="7" t="str">
         <f>IFERROR(SEARCH(K$1,$I44),"")</f>
@@ -7376,33 +7353,31 @@
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>77</v>
+      <c r="A45" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="B45" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C45" s="5">
         <v>7</v>
       </c>
       <c r="D45" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E45" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F45" s="5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G45" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H45" s="5">
-        <v>4</v>
-      </c>
-      <c r="I45" s="7" t="s">
-        <v>4</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I45" s="7"/>
       <c r="J45" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I45),"")</f>
         <v/>
@@ -7415,9 +7390,9 @@
         <f>IFERROR(SEARCH(L$1,$I45),"")</f>
         <v/>
       </c>
-      <c r="M45" s="7">
+      <c r="M45" s="7" t="str">
         <f>IFERROR(SEARCH(M$1,$I45),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="N45" s="7" t="str">
         <f>IFERROR(SEARCH(N$1,$I45),"")</f>
@@ -7433,36 +7408,36 @@
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>78</v>
+      <c r="A46" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="B46" s="5">
         <v>2</v>
       </c>
       <c r="C46" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D46" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E46" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F46" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G46" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H46" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
       <c r="J46" s="7">
         <f>IFERROR(SEARCH(J$1,$I46),"")</f>
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="K46" s="7" t="str">
         <f>IFERROR(SEARCH(K$1,$I46),"")</f>
@@ -7472,9 +7447,9 @@
         <f>IFERROR(SEARCH(L$1,$I46),"")</f>
         <v/>
       </c>
-      <c r="M46" s="7">
+      <c r="M46" s="7" t="str">
         <f>IFERROR(SEARCH(M$1,$I46),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="N46" s="7" t="str">
         <f>IFERROR(SEARCH(N$1,$I46),"")</f>
@@ -7484,37 +7459,39 @@
         <f>IFERROR(SEARCH(O$1,$I46),"")</f>
         <v/>
       </c>
-      <c r="P46" s="7" t="str">
+      <c r="P46" s="7">
         <f>IFERROR(SEARCH(P$1,$I46),"")</f>
-        <v/>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>80</v>
+      <c r="A47" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="B47" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C47" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D47" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E47" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F47" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G47" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H47" s="5">
         <v>1</v>
       </c>
-      <c r="I47" s="7"/>
+      <c r="I47" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="J47" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I47),"")</f>
         <v/>
@@ -7539,42 +7516,40 @@
         <f>IFERROR(SEARCH(O$1,$I47),"")</f>
         <v/>
       </c>
-      <c r="P47" s="7" t="str">
+      <c r="P47" s="7">
         <f>IFERROR(SEARCH(P$1,$I47),"")</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>89</v>
+      <c r="A48" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="B48" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C48" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D48" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E48" s="5">
         <v>5</v>
       </c>
       <c r="F48" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G48" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H48" s="5">
-        <v>2</v>
-      </c>
-      <c r="I48" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J48" s="7">
+        <v>3</v>
+      </c>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I48),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="K48" s="7" t="str">
         <f>IFERROR(SEARCH(K$1,$I48),"")</f>
@@ -7596,37 +7571,39 @@
         <f>IFERROR(SEARCH(O$1,$I48),"")</f>
         <v/>
       </c>
-      <c r="P48" s="7">
+      <c r="P48" s="7" t="str">
         <f>IFERROR(SEARCH(P$1,$I48),"")</f>
-        <v>15</v>
+        <v/>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>9</v>
+      <c r="A49" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="B49" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C49" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D49" s="5">
         <v>7</v>
       </c>
       <c r="E49" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F49" s="5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G49" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H49" s="5">
-        <v>4</v>
-      </c>
-      <c r="I49" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="J49" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I49),"")</f>
         <v/>
@@ -7639,9 +7616,9 @@
         <f>IFERROR(SEARCH(L$1,$I49),"")</f>
         <v/>
       </c>
-      <c r="M49" s="7" t="str">
+      <c r="M49" s="7">
         <f>IFERROR(SEARCH(M$1,$I49),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="N49" s="7" t="str">
         <f>IFERROR(SEARCH(N$1,$I49),"")</f>
@@ -7657,31 +7634,33 @@
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>25</v>
+      <c r="A50" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="B50" s="5">
         <v>4</v>
       </c>
       <c r="C50" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D50" s="5">
         <v>7</v>
       </c>
       <c r="E50" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F50" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G50" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H50" s="5">
         <v>2</v>
       </c>
-      <c r="I50" s="7"/>
+      <c r="I50" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="J50" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I50),"")</f>
         <v/>
@@ -7694,9 +7673,9 @@
         <f>IFERROR(SEARCH(L$1,$I50),"")</f>
         <v/>
       </c>
-      <c r="M50" s="7" t="str">
+      <c r="M50" s="7">
         <f>IFERROR(SEARCH(M$1,$I50),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="N50" s="7" t="str">
         <f>IFERROR(SEARCH(N$1,$I50),"")</f>
@@ -7712,31 +7691,33 @@
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>27</v>
+      <c r="A51" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="B51" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C51" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D51" s="5">
         <v>7</v>
       </c>
       <c r="E51" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F51" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G51" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H51" s="5">
-        <v>5</v>
-      </c>
-      <c r="I51" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="J51" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I51),"")</f>
         <v/>
@@ -7757,9 +7738,9 @@
         <f>IFERROR(SEARCH(N$1,$I51),"")</f>
         <v/>
       </c>
-      <c r="O51" s="7" t="str">
+      <c r="O51" s="7">
         <f>IFERROR(SEARCH(O$1,$I51),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="P51" s="7" t="str">
         <f>IFERROR(SEARCH(P$1,$I51),"")</f>
@@ -7767,29 +7748,29 @@
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
-        <v>29</v>
+      <c r="A52" s="11" t="s">
+        <v>81</v>
       </c>
       <c r="B52" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C52" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D52" s="5">
         <v>7</v>
       </c>
       <c r="E52" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F52" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G52" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H52" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I52" s="7"/>
       <c r="J52" s="7" t="str">
@@ -7822,29 +7803,29 @@
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
-        <v>33</v>
+      <c r="A53" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="B53" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C53" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D53" s="5">
         <v>7</v>
       </c>
       <c r="E53" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F53" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G53" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H53" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I53" s="7"/>
       <c r="J53" s="7" t="str">
@@ -7877,36 +7858,36 @@
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>36</v>
+      <c r="A54" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="B54" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C54" s="5">
         <v>3</v>
       </c>
       <c r="D54" s="5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E54" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F54" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G54" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H54" s="5">
         <v>6</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J54" s="7">
+        <v>4</v>
+      </c>
+      <c r="J54" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I54),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="K54" s="7" t="str">
         <f>IFERROR(SEARCH(K$1,$I54),"")</f>
@@ -7916,9 +7897,9 @@
         <f>IFERROR(SEARCH(L$1,$I54),"")</f>
         <v/>
       </c>
-      <c r="M54" s="7" t="str">
+      <c r="M54" s="7">
         <f>IFERROR(SEARCH(M$1,$I54),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="N54" s="7" t="str">
         <f>IFERROR(SEARCH(N$1,$I54),"")</f>
@@ -7934,33 +7915,31 @@
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
-        <v>37</v>
+      <c r="A55" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="B55" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C55" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D55" s="5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E55" s="5">
         <v>4</v>
       </c>
       <c r="F55" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G55" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H55" s="5">
-        <v>3</v>
-      </c>
-      <c r="I55" s="7" t="s">
-        <v>5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I55" s="7"/>
       <c r="J55" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I55),"")</f>
         <v/>
@@ -7977,9 +7956,9 @@
         <f>IFERROR(SEARCH(M$1,$I55),"")</f>
         <v/>
       </c>
-      <c r="N55" s="7">
+      <c r="N55" s="7" t="str">
         <f>IFERROR(SEARCH(N$1,$I55),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="O55" s="7" t="str">
         <f>IFERROR(SEARCH(O$1,$I55),"")</f>
@@ -7991,40 +7970,38 @@
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
-        <v>42</v>
+      <c r="A56" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="B56" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C56" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D56" s="5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E56" s="5">
         <v>6</v>
       </c>
       <c r="F56" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G56" s="5">
         <v>5</v>
       </c>
       <c r="H56" s="5">
-        <v>1</v>
-      </c>
-      <c r="I56" s="7" t="s">
-        <v>43</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I56" s="7"/>
       <c r="J56" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I56),"")</f>
         <v/>
       </c>
-      <c r="K56" s="7">
+      <c r="K56" s="7" t="str">
         <f>IFERROR(SEARCH(K$1,$I56),"")</f>
-        <v>12</v>
+        <v/>
       </c>
       <c r="L56" s="7" t="str">
         <f>IFERROR(SEARCH(L$1,$I56),"")</f>
@@ -8042,32 +8019,32 @@
         <f>IFERROR(SEARCH(O$1,$I56),"")</f>
         <v/>
       </c>
-      <c r="P56" s="7">
+      <c r="P56" s="7" t="str">
         <f>IFERROR(SEARCH(P$1,$I56),"")</f>
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
-        <v>46</v>
+      <c r="A57" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="B57" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C57" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D57" s="5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E57" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F57" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G57" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H57" s="5">
         <v>2</v>
@@ -8103,36 +8080,36 @@
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
-        <v>48</v>
+      <c r="A58" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="B58" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C58" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D58" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E58" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G58" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H58" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="J58" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="J58" s="7">
         <f>IFERROR(SEARCH(J$1,$I58),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="K58" s="7" t="str">
         <f>IFERROR(SEARCH(K$1,$I58),"")</f>
@@ -8146,9 +8123,9 @@
         <f>IFERROR(SEARCH(M$1,$I58),"")</f>
         <v/>
       </c>
-      <c r="N58" s="7">
+      <c r="N58" s="7" t="str">
         <f>IFERROR(SEARCH(N$1,$I58),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="O58" s="7" t="str">
         <f>IFERROR(SEARCH(O$1,$I58),"")</f>
@@ -8160,33 +8137,31 @@
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
-        <v>49</v>
+      <c r="A59" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="B59" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C59" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D59" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E59" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F59" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G59" s="5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H59" s="5">
-        <v>3</v>
-      </c>
-      <c r="I59" s="7" t="s">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="I59" s="7"/>
       <c r="J59" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I59),"")</f>
         <v/>
@@ -8199,9 +8174,9 @@
         <f>IFERROR(SEARCH(L$1,$I59),"")</f>
         <v/>
       </c>
-      <c r="M59" s="7">
+      <c r="M59" s="7" t="str">
         <f>IFERROR(SEARCH(M$1,$I59),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="N59" s="7" t="str">
         <f>IFERROR(SEARCH(N$1,$I59),"")</f>
@@ -8217,29 +8192,29 @@
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
-        <v>51</v>
+      <c r="A60" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="B60" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C60" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D60" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E60" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F60" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G60" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H60" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I60" s="7"/>
       <c r="J60" s="7" t="str">
@@ -8272,29 +8247,29 @@
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
-        <v>53</v>
+      <c r="A61" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="B61" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C61" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D61" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E61" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F61" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G61" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H61" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I61" s="7"/>
       <c r="J61" s="7" t="str">
@@ -8327,33 +8302,31 @@
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
-        <v>59</v>
+      <c r="A62" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="B62" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C62" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D62" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E62" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F62" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G62" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H62" s="5">
-        <v>2</v>
-      </c>
-      <c r="I62" s="7" t="s">
-        <v>4</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I62" s="7"/>
       <c r="J62" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I62),"")</f>
         <v/>
@@ -8366,9 +8339,9 @@
         <f>IFERROR(SEARCH(L$1,$I62),"")</f>
         <v/>
       </c>
-      <c r="M62" s="7">
+      <c r="M62" s="7" t="str">
         <f>IFERROR(SEARCH(M$1,$I62),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="N62" s="7" t="str">
         <f>IFERROR(SEARCH(N$1,$I62),"")</f>
@@ -8384,38 +8357,40 @@
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
-        <v>60</v>
+      <c r="A63" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="B63" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C63" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D63" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E63" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F63" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G63" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H63" s="5">
-        <v>2</v>
-      </c>
-      <c r="I63" s="7"/>
+        <v>6</v>
+      </c>
+      <c r="I63" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="J63" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I63),"")</f>
         <v/>
       </c>
-      <c r="K63" s="7" t="str">
+      <c r="K63" s="7">
         <f>IFERROR(SEARCH(K$1,$I63),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L63" s="7" t="str">
         <f>IFERROR(SEARCH(L$1,$I63),"")</f>
@@ -8439,40 +8414,40 @@
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
-        <v>63</v>
+      <c r="A64" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="B64" s="5">
         <v>3</v>
       </c>
       <c r="C64" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D64" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E64" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F64" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G64" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H64" s="5">
         <v>2</v>
       </c>
       <c r="I64" s="7" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="J64" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I64),"")</f>
         <v/>
       </c>
-      <c r="K64" s="7" t="str">
+      <c r="K64" s="7">
         <f>IFERROR(SEARCH(K$1,$I64),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L64" s="7" t="str">
         <f>IFERROR(SEARCH(L$1,$I64),"")</f>
@@ -8486,39 +8461,39 @@
         <f>IFERROR(SEARCH(N$1,$I64),"")</f>
         <v/>
       </c>
-      <c r="O64" s="7">
+      <c r="O64" s="7" t="str">
         <f>IFERROR(SEARCH(O$1,$I64),"")</f>
-        <v>1</v>
-      </c>
-      <c r="P64" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P64" s="7">
         <f>IFERROR(SEARCH(P$1,$I64),"")</f>
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
-        <v>66</v>
+      <c r="A65" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="B65" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C65" s="5">
         <v>4</v>
       </c>
       <c r="D65" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E65" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G65" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H65" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I65" s="7"/>
       <c r="J65" s="7" t="str">
@@ -8551,34 +8526,36 @@
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
-        <v>68</v>
+      <c r="A66" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="B66" s="5">
         <v>2</v>
       </c>
       <c r="C66" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D66" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E66" s="5">
         <v>3</v>
       </c>
       <c r="F66" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G66" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H66" s="5">
-        <v>5</v>
-      </c>
-      <c r="I66" s="7"/>
-      <c r="J66" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="I66" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J66" s="7">
         <f>IFERROR(SEARCH(J$1,$I66),"")</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="K66" s="7" t="str">
         <f>IFERROR(SEARCH(K$1,$I66),"")</f>
@@ -8600,35 +8577,35 @@
         <f>IFERROR(SEARCH(O$1,$I66),"")</f>
         <v/>
       </c>
-      <c r="P66" s="7" t="str">
+      <c r="P66" s="7">
         <f>IFERROR(SEARCH(P$1,$I66),"")</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
-        <v>73</v>
+      <c r="A67" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="B67" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C67" s="5">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D67" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E67" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F67" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G67" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H67" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I67" s="7"/>
       <c r="J67" s="7" t="str">
@@ -8661,31 +8638,33 @@
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
-        <v>81</v>
+      <c r="A68" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="B68" s="5">
         <v>5</v>
       </c>
       <c r="C68" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D68" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E68" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F68" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G68" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H68" s="5">
-        <v>3</v>
-      </c>
-      <c r="I68" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="I68" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="J68" s="7" t="str">
         <f>IFERROR(SEARCH(J$1,$I68),"")</f>
         <v/>
@@ -8710,35 +8689,35 @@
         <f>IFERROR(SEARCH(O$1,$I68),"")</f>
         <v/>
       </c>
-      <c r="P68" s="7" t="str">
+      <c r="P68" s="7">
         <f>IFERROR(SEARCH(P$1,$I68),"")</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
-        <v>82</v>
+      <c r="A69" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="B69" s="5">
         <v>5</v>
       </c>
       <c r="C69" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D69" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E69" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F69" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G69" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H69" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I69" s="7"/>
       <c r="J69" s="7" t="str">
@@ -8771,29 +8750,29 @@
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
-        <v>86</v>
+      <c r="A70" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="B70" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C70" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D70" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E70" s="5">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F70" s="5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G70" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H70" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I70" s="7"/>
       <c r="J70" s="7" t="str">
@@ -8826,29 +8805,29 @@
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
-        <v>88</v>
+      <c r="A71" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="B71" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C71" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D71" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E71" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F71" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G71" s="5">
         <v>5</v>
       </c>
       <c r="H71" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I71" s="7"/>
       <c r="J71" s="7" t="str">
@@ -8881,7 +8860,7 @@
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="12" t="s">
         <v>92</v>
       </c>
       <c r="B73" s="3">
@@ -8889,32 +8868,32 @@
         <v>3.7714285714285714</v>
       </c>
       <c r="C73" s="3">
-        <f t="shared" ref="C73:H73" si="0">AVERAGE(C2:C71)</f>
+        <f>AVERAGE(C2:C71)</f>
         <v>4.0571428571428569</v>
       </c>
       <c r="D73" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D2:D71)</f>
         <v>4.8571428571428568</v>
       </c>
       <c r="E73" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(E2:E71)</f>
         <v>3.6</v>
       </c>
       <c r="F73" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(F2:F71)</f>
         <v>4.3571428571428568</v>
       </c>
       <c r="G73" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(G2:G71)</f>
         <v>3.9</v>
       </c>
       <c r="H73" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(H2:H71)</f>
         <v>3.4571428571428573</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A74" s="4">
+      <c r="A74" s="13">
         <v>1</v>
       </c>
       <c r="B74" s="1">
@@ -8922,99 +8901,99 @@
         <v>8</v>
       </c>
       <c r="C74" s="1">
-        <f t="shared" ref="C74:H74" si="1">COUNTIF(C$2:C$71,$A74)</f>
+        <f>COUNTIF(C$2:C$71,$A74)</f>
         <v>9</v>
       </c>
       <c r="D74" s="1">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(D$2:D$71,$A74)</f>
         <v>6</v>
       </c>
       <c r="E74" s="1">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(E$2:E$71,$A74)</f>
         <v>10</v>
       </c>
       <c r="F74" s="1">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F$2:F$71,$A74)</f>
         <v>19</v>
       </c>
       <c r="G74" s="1">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(G$2:G$71,$A74)</f>
         <v>6</v>
       </c>
       <c r="H74" s="1">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(H$2:H$71,$A74)</f>
         <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A75" s="4">
+      <c r="A75" s="13">
         <v>2</v>
       </c>
       <c r="B75" s="1">
-        <f t="shared" ref="B75:H76" si="2">COUNTIF(B$2:B$71,$A75)</f>
+        <f>COUNTIF(B$2:B$71,$A75)</f>
         <v>9</v>
       </c>
       <c r="C75" s="1">
-        <f t="shared" si="2"/>
+        <f>COUNTIF(C$2:C$71,$A75)</f>
         <v>9</v>
       </c>
       <c r="D75" s="1">
-        <f t="shared" si="2"/>
+        <f>COUNTIF(D$2:D$71,$A75)</f>
         <v>7</v>
       </c>
       <c r="E75" s="1">
-        <f t="shared" si="2"/>
+        <f>COUNTIF(E$2:E$71,$A75)</f>
         <v>10</v>
       </c>
       <c r="F75" s="1">
-        <f t="shared" si="2"/>
+        <f>COUNTIF(F$2:F$71,$A75)</f>
         <v>5</v>
       </c>
       <c r="G75" s="1">
-        <f t="shared" si="2"/>
+        <f>COUNTIF(G$2:G$71,$A75)</f>
         <v>11</v>
       </c>
       <c r="H75" s="1">
-        <f t="shared" si="2"/>
+        <f>COUNTIF(H$2:H$71,$A75)</f>
         <v>19</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A76" s="4">
+      <c r="A76" s="13">
         <v>3</v>
       </c>
       <c r="B76" s="1">
-        <f t="shared" si="2"/>
+        <f>COUNTIF(B$2:B$71,$A76)</f>
         <v>13</v>
       </c>
       <c r="C76" s="1">
-        <f t="shared" si="2"/>
+        <f>COUNTIF(C$2:C$71,$A76)</f>
         <v>8</v>
       </c>
       <c r="D76" s="1">
-        <f t="shared" si="2"/>
+        <f>COUNTIF(D$2:D$71,$A76)</f>
         <v>6</v>
       </c>
       <c r="E76" s="1">
-        <f t="shared" si="2"/>
+        <f>COUNTIF(E$2:E$71,$A76)</f>
         <v>18</v>
       </c>
       <c r="F76" s="1">
-        <f t="shared" si="2"/>
+        <f>COUNTIF(F$2:F$71,$A76)</f>
         <v>4</v>
       </c>
       <c r="G76" s="1">
-        <f t="shared" si="2"/>
+        <f>COUNTIF(G$2:G$71,$A76)</f>
         <v>11</v>
       </c>
       <c r="H76" s="1">
-        <f t="shared" si="2"/>
+        <f>COUNTIF(H$2:H$71,$A76)</f>
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:P71">
-    <sortCondition ref="D2:D71"/>
+  <sortState ref="A13:P71">
+    <sortCondition ref="F12:F71"/>
   </sortState>
   <conditionalFormatting sqref="J2:P71">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
@@ -9022,5 +9001,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>